<commit_message>
fix on excel file
</commit_message>
<xml_diff>
--- a/assign1/doc/Resultados CPD Projeto1.xlsx
+++ b/assign1/doc/Resultados CPD Projeto1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnemberg/Desktop/3ºano/CPD/g11/assign1/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FBC7BD-F4F7-4549-801C-DD99ECF43014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010E4B99-7A4C-9C4A-901A-27757A7C8A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,67 +560,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>965199</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>120972</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A5BDC7E-6DD1-4A28-E636-C65C899CF397}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6756399" y="0"/>
-          <a:ext cx="5912173" cy="3619499"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
@@ -646,7 +585,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -707,7 +646,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -768,7 +707,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -829,7 +768,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -890,7 +829,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -951,7 +890,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1012,7 +951,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1028,6 +967,67 @@
         <a:xfrm>
           <a:off x="14478000" y="9144000"/>
           <a:ext cx="6235700" cy="3855741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>965199</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>863324</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3134C0C0-2B02-4BA6-323E-555E4BBCF0D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6756399" y="190500"/>
+          <a:ext cx="5689325" cy="3517900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7147,17 +7147,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W32:AA32"/>
-    <mergeCell ref="AD32:AH32"/>
-    <mergeCell ref="I47:M47"/>
-    <mergeCell ref="P47:T47"/>
-    <mergeCell ref="W47:AA47"/>
-    <mergeCell ref="P55:T55"/>
-    <mergeCell ref="W55:AA55"/>
-    <mergeCell ref="I63:M63"/>
-    <mergeCell ref="P63:T63"/>
-    <mergeCell ref="W63:AA63"/>
-    <mergeCell ref="I55:M55"/>
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="P2:T2"/>
     <mergeCell ref="W2:AA2"/>
@@ -7166,6 +7155,17 @@
     <mergeCell ref="P17:T17"/>
     <mergeCell ref="AD17:AH17"/>
     <mergeCell ref="W17:AA17"/>
+    <mergeCell ref="P55:T55"/>
+    <mergeCell ref="W55:AA55"/>
+    <mergeCell ref="I63:M63"/>
+    <mergeCell ref="P63:T63"/>
+    <mergeCell ref="W63:AA63"/>
+    <mergeCell ref="I55:M55"/>
+    <mergeCell ref="W32:AA32"/>
+    <mergeCell ref="AD32:AH32"/>
+    <mergeCell ref="I47:M47"/>
+    <mergeCell ref="P47:T47"/>
+    <mergeCell ref="W47:AA47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7178,8 +7178,8 @@
   </sheetPr>
   <dimension ref="F1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T76" sqref="T76"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>